<commit_message>
Retraitement spécifique du poste de certains joueurs, et bascule des joueurs out en bas du TI
</commit_message>
<xml_diff>
--- a/Excel/Impact_poste/Impact_poste_2024_02_29.xlsx
+++ b/Excel/Impact_poste/Impact_poste_2024_02_29.xlsx
@@ -470,10 +470,10 @@
         <v>-3.099999999999998</v>
       </c>
       <c r="C2" t="n">
-        <v>-3.700000000000003</v>
+        <v>-3.900000000000002</v>
       </c>
       <c r="D2" t="n">
-        <v>-4.400000000000002</v>
+        <v>-4.099999999999998</v>
       </c>
       <c r="E2" t="n">
         <v>-2.600000000000001</v>
@@ -489,10 +489,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>4</v>
+        <v>4.099999999999998</v>
       </c>
       <c r="D3" t="n">
-        <v>3.399999999999999</v>
+        <v>3.5</v>
       </c>
       <c r="E3" t="n">
         <v>2.199999999999999</v>
@@ -508,10 +508,10 @@
         <v>1.800000000000001</v>
       </c>
       <c r="C4" t="n">
-        <v>3</v>
+        <v>2.699999999999999</v>
       </c>
       <c r="D4" t="n">
-        <v>1.599999999999998</v>
+        <v>2</v>
       </c>
       <c r="E4" t="n">
         <v>2.100000000000001</v>
@@ -527,10 +527,10 @@
         <v>0.6999999999999993</v>
       </c>
       <c r="C5" t="n">
-        <v>0.5999999999999979</v>
+        <v>0.3999999999999986</v>
       </c>
       <c r="D5" t="n">
-        <v>-1.100000000000001</v>
+        <v>-0.8999999999999986</v>
       </c>
       <c r="E5" t="n">
         <v>0.1999999999999993</v>
@@ -546,10 +546,10 @@
         <v>-1</v>
       </c>
       <c r="C6" t="n">
-        <v>-3.700000000000003</v>
+        <v>-3.900000000000002</v>
       </c>
       <c r="D6" t="n">
-        <v>-2</v>
+        <v>-1.799999999999997</v>
       </c>
       <c r="E6" t="n">
         <v>-2.199999999999999</v>
@@ -565,10 +565,10 @@
         <v>-0.1999999999999993</v>
       </c>
       <c r="C7" t="n">
-        <v>0.5999999999999979</v>
+        <v>0.8000000000000007</v>
       </c>
       <c r="D7" t="n">
-        <v>2.5</v>
+        <v>2.200000000000003</v>
       </c>
       <c r="E7" t="n">
         <v>0.5</v>
@@ -584,10 +584,10 @@
         <v>-0.8999999999999986</v>
       </c>
       <c r="C8" t="n">
-        <v>1.199999999999999</v>
+        <v>1.099999999999998</v>
       </c>
       <c r="D8" t="n">
-        <v>0.2999999999999972</v>
+        <v>0.3000000000000007</v>
       </c>
       <c r="E8" t="n">
         <v>0.1000000000000014</v>
@@ -603,10 +603,10 @@
         <v>-1.300000000000001</v>
       </c>
       <c r="C9" t="n">
-        <v>-1.100000000000001</v>
+        <v>-1.199999999999999</v>
       </c>
       <c r="D9" t="n">
-        <v>-2.400000000000002</v>
+        <v>-2.299999999999997</v>
       </c>
       <c r="E9" t="n">
         <v>-1.5</v>
@@ -622,10 +622,10 @@
         <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>-0.1999999999999993</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.1000000000000014</v>
+        <v>0.2000000000000028</v>
       </c>
       <c r="E10" t="n">
         <v>0.3999999999999986</v>
@@ -641,10 +641,10 @@
         <v>-1.800000000000001</v>
       </c>
       <c r="C11" t="n">
-        <v>-1.900000000000002</v>
+        <v>-1.699999999999999</v>
       </c>
       <c r="D11" t="n">
-        <v>0.5</v>
+        <v>0.2000000000000028</v>
       </c>
       <c r="E11" t="n">
         <v>-1.5</v>
@@ -663,7 +663,7 @@
         <v>1.699999999999999</v>
       </c>
       <c r="D12" t="n">
-        <v>2.099999999999998</v>
+        <v>2.100000000000001</v>
       </c>
       <c r="E12" t="n">
         <v>1.699999999999999</v>
@@ -679,10 +679,10 @@
         <v>1.300000000000001</v>
       </c>
       <c r="C13" t="n">
-        <v>0.3999999999999986</v>
+        <v>0.3000000000000007</v>
       </c>
       <c r="D13" t="n">
-        <v>1.5</v>
+        <v>1.800000000000001</v>
       </c>
       <c r="E13" t="n">
         <v>1.100000000000001</v>
@@ -698,10 +698,10 @@
         <v>-0.09999999999999787</v>
       </c>
       <c r="C14" t="n">
-        <v>-1.300000000000001</v>
+        <v>-1.5</v>
       </c>
       <c r="D14" t="n">
-        <v>0.3999999999999986</v>
+        <v>0.7000000000000028</v>
       </c>
       <c r="E14" t="n">
         <v>-0.3999999999999986</v>
@@ -717,10 +717,10 @@
         <v>2</v>
       </c>
       <c r="C15" t="n">
-        <v>4</v>
+        <v>4.099999999999998</v>
       </c>
       <c r="D15" t="n">
-        <v>-0.4000000000000021</v>
+        <v>-0.6999999999999993</v>
       </c>
       <c r="E15" t="n">
         <v>2.199999999999999</v>
@@ -739,7 +739,7 @@
         <v>-1.900000000000002</v>
       </c>
       <c r="D16" t="n">
-        <v>-2.100000000000001</v>
+        <v>-2.199999999999999</v>
       </c>
       <c r="E16" t="n">
         <v>-1.300000000000001</v>
@@ -777,7 +777,7 @@
         <v>0.5999999999999979</v>
       </c>
       <c r="D18" t="n">
-        <v>0.5999999999999979</v>
+        <v>0.5</v>
       </c>
       <c r="E18" t="n">
         <v>-0.1000000000000014</v>
@@ -793,10 +793,10 @@
         <v>0.3000000000000007</v>
       </c>
       <c r="C19" t="n">
-        <v>-0.5</v>
+        <v>-0.8000000000000007</v>
       </c>
       <c r="D19" t="n">
-        <v>-4.400000000000002</v>
+        <v>-4.099999999999998</v>
       </c>
       <c r="E19" t="n">
         <v>-0.8999999999999986</v>
@@ -815,7 +815,7 @@
         <v>-1.600000000000001</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.4000000000000021</v>
+        <v>-0.2999999999999972</v>
       </c>
       <c r="E20" t="n">
         <v>0.1999999999999993</v>
@@ -831,10 +831,10 @@
         <v>-3.099999999999998</v>
       </c>
       <c r="C21" t="n">
-        <v>-2.200000000000003</v>
+        <v>-2.300000000000001</v>
       </c>
       <c r="D21" t="n">
-        <v>-2.200000000000003</v>
+        <v>-2</v>
       </c>
       <c r="E21" t="n">
         <v>-2.600000000000001</v>
@@ -850,10 +850,10 @@
         <v>-1.800000000000001</v>
       </c>
       <c r="C22" t="n">
-        <v>-2.700000000000003</v>
+        <v>-2.800000000000001</v>
       </c>
       <c r="D22" t="n">
-        <v>-1.5</v>
+        <v>-1.299999999999997</v>
       </c>
       <c r="E22" t="n">
         <v>-1.899999999999999</v>
@@ -869,10 +869,10 @@
         <v>-1.300000000000001</v>
       </c>
       <c r="C23" t="n">
-        <v>0.09999999999999787</v>
+        <v>-0.1000000000000014</v>
       </c>
       <c r="D23" t="n">
-        <v>-4.100000000000001</v>
+        <v>-3.899999999999999</v>
       </c>
       <c r="E23" t="n">
         <v>-1.399999999999999</v>
@@ -888,10 +888,10 @@
         <v>-2.099999999999998</v>
       </c>
       <c r="C24" t="n">
-        <v>-1.800000000000001</v>
+        <v>-1.5</v>
       </c>
       <c r="D24" t="n">
-        <v>1.5</v>
+        <v>1.100000000000001</v>
       </c>
       <c r="E24" t="n">
         <v>-1.300000000000001</v>
@@ -907,10 +907,10 @@
         <v>0.1000000000000014</v>
       </c>
       <c r="C25" t="n">
-        <v>-2.300000000000001</v>
+        <v>-2.400000000000002</v>
       </c>
       <c r="D25" t="n">
-        <v>-1</v>
+        <v>-0.7999999999999972</v>
       </c>
       <c r="E25" t="n">
         <v>-0.8000000000000007</v>
@@ -926,10 +926,10 @@
         <v>0.1000000000000014</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.5</v>
+        <v>-0.1999999999999993</v>
       </c>
       <c r="D26" t="n">
-        <v>-0.1000000000000014</v>
+        <v>-0.5999999999999979</v>
       </c>
       <c r="E26" t="n">
         <v>-0.1000000000000014</v>
@@ -945,10 +945,10 @@
         <v>-0.5</v>
       </c>
       <c r="C27" t="n">
-        <v>-0.5</v>
+        <v>-0.1000000000000014</v>
       </c>
       <c r="D27" t="n">
-        <v>0.6999999999999993</v>
+        <v>0.4000000000000021</v>
       </c>
       <c r="E27" t="n">
         <v>-0.1999999999999993</v>
@@ -964,10 +964,10 @@
         <v>-0.09999999999999787</v>
       </c>
       <c r="C28" t="n">
-        <v>-0.3000000000000007</v>
+        <v>-0.4000000000000021</v>
       </c>
       <c r="D28" t="n">
-        <v>2.899999999999999</v>
+        <v>3.100000000000001</v>
       </c>
       <c r="E28" t="n">
         <v>0.5</v>
@@ -983,10 +983,10 @@
         <v>1.800000000000001</v>
       </c>
       <c r="C29" t="n">
-        <v>2.099999999999998</v>
+        <v>2</v>
       </c>
       <c r="D29" t="n">
-        <v>-1.5</v>
+        <v>-1.299999999999997</v>
       </c>
       <c r="E29" t="n">
         <v>1.199999999999999</v>
@@ -1002,10 +1002,10 @@
         <v>0.6999999999999993</v>
       </c>
       <c r="C30" t="n">
-        <v>0.7999999999999972</v>
+        <v>1</v>
       </c>
       <c r="D30" t="n">
-        <v>2.5</v>
+        <v>2.200000000000003</v>
       </c>
       <c r="E30" t="n">
         <v>1.100000000000001</v>
@@ -1021,10 +1021,10 @@
         <v>1</v>
       </c>
       <c r="C31" t="n">
-        <v>0.1999999999999993</v>
+        <v>0.3999999999999986</v>
       </c>
       <c r="D31" t="n">
-        <v>1.299999999999997</v>
+        <v>1.100000000000001</v>
       </c>
       <c r="E31" t="n">
         <v>0.8000000000000007</v>
@@ -1040,10 +1040,10 @@
         <v>0.1000000000000014</v>
       </c>
       <c r="C32" t="n">
-        <v>2.799999999999997</v>
+        <v>2.599999999999998</v>
       </c>
       <c r="D32" t="n">
-        <v>0</v>
+        <v>0.2000000000000028</v>
       </c>
       <c r="E32" t="n">
         <v>0.8999999999999986</v>
@@ -1059,10 +1059,10 @@
         <v>0.8000000000000007</v>
       </c>
       <c r="C33" t="n">
-        <v>2.399999999999999</v>
+        <v>2.300000000000001</v>
       </c>
       <c r="D33" t="n">
-        <v>3.399999999999999</v>
+        <v>3.5</v>
       </c>
       <c r="E33" t="n">
         <v>1.800000000000001</v>

</xml_diff>